<commit_message>
corrections for test run
</commit_message>
<xml_diff>
--- a/docs/Gewicht Eichung Loadcell.xlsx
+++ b/docs/Gewicht Eichung Loadcell.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\beehive-sensor\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB1ACA3-0813-4C80-853D-A7C185A82551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DE676A-5311-444C-8616-F6449E8E087F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8B69D70C-2B63-46EE-9209-063377342C58}"/>
   </bookViews>
@@ -58,15 +58,6 @@
   </si>
   <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>Stock 1</t>
-  </si>
-  <si>
-    <t>Stock 2</t>
-  </si>
-  <si>
-    <t>Stock 3</t>
   </si>
   <si>
     <t>Cell Reading</t>
@@ -130,6 +121,15 @@
   </si>
   <si>
     <t>T-OFFSET</t>
+  </si>
+  <si>
+    <t>Krokus</t>
+  </si>
+  <si>
+    <t>Shakra</t>
+  </si>
+  <si>
+    <t>Gotthard</t>
   </si>
 </sst>
 </file>
@@ -274,12 +274,12 @@
     <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -3893,7 +3893,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3911,23 +3911,23 @@
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="B1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="F1" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
       <c r="I1" s="3"/>
-      <c r="J1" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="J1" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4110,7 +4110,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="21">
@@ -4133,7 +4133,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="21">
@@ -4185,7 +4185,7 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4197,7 +4197,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -4208,42 +4208,42 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H2" s="15"/>
       <c r="Q2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
         <v>-43496</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="22">
         <v>20</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="23">
         <v>0</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="24">
         <f t="shared" ref="D3:D10" si="0">(A3-$T$5)/$T$4</f>
         <v>2.0434399999988672E-4</v>
       </c>
@@ -4251,7 +4251,7 @@
         <f>D3-C3</f>
         <v>2.0434399999988672E-4</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="24">
         <f t="shared" ref="F3:F10" si="1">D3-$R$19*B3-$R$20</f>
         <v>-4.8496560000001118E-3</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>-4.8496560000001118E-3</v>
       </c>
       <c r="Q3" s="20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R3" s="20"/>
       <c r="S3" s="20"/>
@@ -4270,13 +4270,13 @@
       <c r="A4" s="17">
         <v>108691</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="22">
         <v>20</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="23">
         <v>6</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="24">
         <f t="shared" si="0"/>
         <v>6.0056555510000003</v>
       </c>
@@ -4284,7 +4284,7 @@
         <f t="shared" ref="E4:E10" si="2">D4-C4</f>
         <v>5.6555510000002585E-3</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="24">
         <f t="shared" si="1"/>
         <v>6.0006015509999999</v>
       </c>
@@ -4293,13 +4293,13 @@
         <v>6.0155099999992245E-4</v>
       </c>
       <c r="Q4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="R4" s="19">
         <v>3.9461E-5</v>
       </c>
       <c r="S4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="T4" s="13">
         <f>1/R4</f>
@@ -4310,13 +4310,13 @@
       <c r="A5" s="18">
         <v>108000</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="22">
         <v>0</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="23">
         <v>6</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="24">
         <f t="shared" si="0"/>
         <v>5.9783880000000007</v>
       </c>
@@ -4324,7 +4324,7 @@
         <f t="shared" si="2"/>
         <v>-2.1611999999999298E-2</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="24">
         <f t="shared" si="1"/>
         <v>5.9983820000000003</v>
       </c>
@@ -4333,13 +4333,13 @@
         <v>-1.6179999999996753E-3</v>
       </c>
       <c r="Q5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="R5" s="19">
         <v>1.7165999999999999</v>
       </c>
       <c r="S5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T5" s="13">
         <f>-T4*R5</f>
@@ -4350,13 +4350,13 @@
       <c r="A6" s="18">
         <v>109000</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="22">
         <v>30</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="23">
         <v>6</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="24">
         <f t="shared" si="0"/>
         <v>6.017849</v>
       </c>
@@ -4364,7 +4364,7 @@
         <f t="shared" si="2"/>
         <v>1.7849000000000004E-2</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="24">
         <f t="shared" si="1"/>
         <v>6.0002709999999997</v>
       </c>
@@ -4377,13 +4377,13 @@
       <c r="A7" s="18">
         <v>108500</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="22">
         <v>10</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="23">
         <v>6</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="24">
         <f t="shared" si="0"/>
         <v>5.9981185000000004</v>
       </c>
@@ -4391,7 +4391,7 @@
         <f t="shared" si="2"/>
         <v>-1.8814999999996473E-3</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="24">
         <f t="shared" si="1"/>
         <v>6.0055885</v>
       </c>
@@ -4404,13 +4404,13 @@
       <c r="A8" s="18">
         <v>-43000</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B8" s="22">
         <v>30</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="23">
         <v>0</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="24">
         <f t="shared" si="0"/>
         <v>1.9776999999999888E-2</v>
       </c>
@@ -4418,7 +4418,7 @@
         <f t="shared" si="2"/>
         <v>1.9776999999999888E-2</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="24">
         <f t="shared" si="1"/>
         <v>2.1989999999998885E-3</v>
       </c>
@@ -4431,13 +4431,13 @@
       <c r="A9" s="18">
         <v>-43500</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="22">
         <v>18</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="23">
         <v>0</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="24">
         <f t="shared" si="0"/>
         <v>4.649999999988672E-5</v>
       </c>
@@ -4445,7 +4445,7 @@
         <f t="shared" si="2"/>
         <v>4.649999999988672E-5</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="24">
         <f t="shared" si="1"/>
         <v>-2.5027000000001146E-3</v>
       </c>
@@ -4458,13 +4458,13 @@
       <c r="A10" s="18">
         <v>-44000</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="22">
         <v>0</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="23">
         <v>0</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="24">
         <f t="shared" si="0"/>
         <v>-1.9684000000000115E-2</v>
       </c>
@@ -4472,7 +4472,7 @@
         <f t="shared" si="2"/>
         <v>-1.9684000000000115E-2</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="24">
         <f t="shared" si="1"/>
         <v>3.0999999999988676E-4</v>
       </c>
@@ -4537,7 +4537,7 @@
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="Q17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
@@ -4548,7 +4548,7 @@
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
       <c r="Q18" s="20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R18" s="20"/>
       <c r="S18" s="20"/>
@@ -4556,7 +4556,7 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="Q19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="R19" s="19">
         <v>1.2524000000000001E-3</v>
@@ -4564,7 +4564,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="Q20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="R20" s="19">
         <v>-1.9994000000000001E-2</v>
@@ -4572,12 +4572,12 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="Q32" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q33" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
additional hints for weight calibration
</commit_message>
<xml_diff>
--- a/docs/Gewicht Eichung Loadcell.xlsx
+++ b/docs/Gewicht Eichung Loadcell.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\beehive-sensor\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DE676A-5311-444C-8616-F6449E8E087F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07313264-02B5-4E36-BD0E-0CA97B41978E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8B69D70C-2B63-46EE-9209-063377342C58}"/>
   </bookViews>
   <sheets>
-    <sheet name="Einzel" sheetId="1" r:id="rId1"/>
-    <sheet name="Statistisch" sheetId="2" r:id="rId2"/>
+    <sheet name="Messungen" sheetId="3" r:id="rId1"/>
+    <sheet name="Auswertung" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,31 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
-  <si>
-    <t>Leergewicht</t>
-  </si>
-  <si>
-    <t>Cell-Reading</t>
-  </si>
-  <si>
-    <t>Gewicht</t>
-  </si>
-  <si>
-    <t>Zustand</t>
-  </si>
-  <si>
-    <t>Belastet</t>
-  </si>
-  <si>
-    <t>OFFSET</t>
-  </si>
-  <si>
-    <t>DIVIDER</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Cell Reading</t>
   </si>
@@ -96,9 +72,6 @@
     <t>Kompensiert</t>
   </si>
   <si>
-    <t>(aus dem Chart in gelbe Felder übertragen)</t>
-  </si>
-  <si>
     <t>(Messungen mit verschiedenen Temperaturen und Gewichten in gelbe Felder eintragen)</t>
   </si>
   <si>
@@ -117,46 +90,29 @@
     <t>sollte nahe bei 0 liegen.</t>
   </si>
   <si>
-    <t>T-FACTOR</t>
+    <t>Label der Trendlinie: y = {M-Factor}x + {M-Offset}</t>
   </si>
   <si>
-    <t>T-OFFSET</t>
+    <t>Aus dem Chart in gelbe Felder übertragen.</t>
   </si>
   <si>
-    <t>Krokus</t>
-  </si>
-  <si>
-    <t>Shakra</t>
-  </si>
-  <si>
-    <t>Gotthard</t>
+    <t>Label der Trendlinie: y = {T-Factor}x + {T-Offset}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="0.00\ &quot;g&quot;"/>
-    <numFmt numFmtId="165" formatCode="0.00\ &quot;kg&quot;"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+  <numFmts count="4">
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="0.0000E+00"/>
     <numFmt numFmtId="169" formatCode="0.0\ &quot;⁰C&quot;"/>
     <numFmt numFmtId="170" formatCode="0.000\ &quot;kg&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -169,30 +125,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -207,28 +145,10 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -243,46 +163,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -378,7 +279,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Statistisch!$C$2</c:f>
+              <c:f>Messungen!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -423,6 +324,12 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.9160104986876643E-3"/>
+                  <c:y val="-0.57207932341790613"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="0.0000E+00" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -453,59 +360,85 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Statistisch!$A$3:$A$99</c:f>
+              <c:f>Messungen!$A$3:$A$89</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="97"/>
+                <c:ptCount val="87"/>
                 <c:pt idx="0">
-                  <c:v>-43496</c:v>
+                  <c:v>-913856</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>108691</c:v>
+                  <c:v>-804510</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>108000</c:v>
+                  <c:v>-806358</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>109000</c:v>
+                  <c:v>-914010</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108500</c:v>
+                  <c:v>-912120</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-43000</c:v>
+                  <c:v>-804830</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-43500</c:v>
+                  <c:v>-805190</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-44000</c:v>
+                  <c:v>-805850</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-805750</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-806910</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-807723</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-808187</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Statistisch!$C$3:$C$99</c:f>
+              <c:f>Messungen!$C$3:$C$89</c:f>
               <c:numCache>
                 <c:formatCode>0.000\ "kg"</c:formatCode>
-                <c:ptCount val="97"/>
+                <c:ptCount val="87"/>
                 <c:pt idx="0">
+                  <c:v>9.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>6</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>9.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>9.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -514,6 +447,18 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -853,7 +798,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Statistisch!$E$2</c:f>
+              <c:f>Messungen!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -894,54 +839,16 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="log"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="0.0000E+00" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.8102799650043747E-2"/>
+                  <c:y val="-0.16896689997083697"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="0.0000E+00" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -974,66 +881,90 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Statistisch!$B$3:$B$99</c:f>
+              <c:f>Messungen!$B$3:$B$89</c:f>
               <c:numCache>
                 <c:formatCode>0.0\ "⁰C"</c:formatCode>
-                <c:ptCount val="97"/>
+                <c:ptCount val="87"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>22.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>11.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>19.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18</c:v>
+                  <c:v>13.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>16.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Statistisch!$E$3:$E$99</c:f>
+              <c:f>Messungen!$E$3:$E$89</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="97"/>
+                <c:ptCount val="87"/>
                 <c:pt idx="0">
-                  <c:v>2.0434399999988672E-4</c:v>
+                  <c:v>4.4390527999990326E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.6555510000002585E-3</c:v>
+                  <c:v>-0.1465823700000099</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.1611999999999298E-2</c:v>
+                  <c:v>2.1424853999990102E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7849000000000004E-2</c:v>
+                  <c:v>5.8391129999989744E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.8814999999996473E-3</c:v>
+                  <c:v>-0.11343444000000957</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.9776999999999888E-2</c:v>
+                  <c:v>-0.11749021000000989</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.649999999988672E-5</c:v>
+                  <c:v>-8.4761530000009896E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.9684000000000115E-2</c:v>
+                  <c:v>-2.4758950000009897E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-3.3850250000009893E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.1608829999990103E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.14552109899999011</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1877047309999901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1397,7 +1328,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Statistisch!$G$2</c:f>
+              <c:f>Messungen!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1444,66 +1375,90 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Statistisch!$B$3:$B$99</c:f>
+              <c:f>Messungen!$B$3:$B$89</c:f>
               <c:numCache>
                 <c:formatCode>0.0\ "⁰C"</c:formatCode>
-                <c:ptCount val="97"/>
+                <c:ptCount val="87"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>22.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>11.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>19.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18</c:v>
+                  <c:v>13.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>16.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Statistisch!$G$3:$G$99</c:f>
+              <c:f>Messungen!$G$3:$G$89</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="97"/>
+                <c:ptCount val="87"/>
                 <c:pt idx="0">
-                  <c:v>-4.8496560000001118E-3</c:v>
+                  <c:v>-8.0659872000008903E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0155099999992245E-4</c:v>
+                  <c:v>-1.0926570000009905E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.6179999999996753E-3</c:v>
+                  <c:v>-2.2304346000009856E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7099999999968816E-4</c:v>
+                  <c:v>-1.1647870000009775E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.5884999999999962E-3</c:v>
+                  <c:v>7.8705599999899789E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1989999999998885E-3</c:v>
+                  <c:v>3.8147899999900758E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-2.5027000000001146E-3</c:v>
+                  <c:v>3.0582699999900931E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0999999999988676E-4</c:v>
+                  <c:v>-1.5177500000099209E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.1335499999901066E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5698299999901133E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.1996898999990151E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.2654330999990071E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3484,13 +3439,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
@@ -3520,13 +3475,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>4762</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>309562</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
@@ -3556,13 +3511,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>4762</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>309562</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
@@ -3889,695 +3844,504 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D23C5679-24D0-491F-B2DA-2E57C3C0BE7F}">
-  <dimension ref="A1:M11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB70EFBE-8999-4967-8E5C-A2958F6E5E70}">
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="1.7109375" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="3"/>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="3"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="9">
-        <v>-43496</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="9">
-        <v>-43496</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="9">
-        <v>-43496</v>
-      </c>
-      <c r="L4" s="5">
-        <v>0</v>
-      </c>
-      <c r="M4" s="3"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5">
-        <v>6</v>
-      </c>
-      <c r="C5" s="9">
-        <v>108691</v>
-      </c>
-      <c r="D5" s="6">
-        <f>D4+B5</f>
-        <v>6</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="5">
-        <v>6</v>
-      </c>
-      <c r="G5" s="9">
-        <v>108691</v>
-      </c>
-      <c r="H5" s="6">
-        <f>H4+F5</f>
-        <v>6</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="5">
-        <v>6</v>
-      </c>
-      <c r="K5" s="9">
-        <v>108691</v>
-      </c>
-      <c r="L5" s="6">
-        <f>L4+J5</f>
-        <v>6</v>
-      </c>
-      <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7">
-        <f>C4-(D4*C10)</f>
-        <v>-43496</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7">
-        <f>G4-(H4*G10)</f>
-        <v>-43496</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7">
-        <f>K4-(L4*K10)</f>
-        <v>-43496</v>
-      </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="3"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7">
-        <f>ROUND((C5-C4)/B5,0)</f>
-        <v>25365</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7">
-        <f>ROUND((G5-G4)/F5,0)</f>
-        <v>25365</v>
-      </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7">
-        <f>ROUND((K5-K4)/J5,0)</f>
-        <v>25365</v>
-      </c>
-      <c r="L8" s="8"/>
-      <c r="M8" s="3"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="21">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="21">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="21">
-        <v>0</v>
-      </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="21">
-        <v>0</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="21">
-        <v>0</v>
-      </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="21">
-        <v>0</v>
-      </c>
-      <c r="L10" s="8"/>
-      <c r="M10" s="3"/>
-    </row>
-    <row r="11" spans="1:13" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="J1:L1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{190CE8A5-5FE3-40A5-93F7-0F18B64AB58A}">
-  <dimension ref="A1:T33"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>-913856</v>
+      </c>
+      <c r="B3" s="12">
+        <v>22.8</v>
+      </c>
+      <c r="C3" s="13">
+        <v>9.75</v>
+      </c>
+      <c r="D3" s="6">
+        <f>(A3-Auswertung!$M$6)/Auswertung!$M$5</f>
+        <v>9.7943905279999903</v>
+      </c>
+      <c r="E3" s="2">
+        <f>D3-C3</f>
+        <v>4.4390527999990326E-2</v>
+      </c>
+      <c r="F3" s="6">
+        <f>D3-Auswertung!$K$20*B3-Auswertung!$K$21</f>
+        <v>9.6693401279999911</v>
+      </c>
+      <c r="G3" s="2">
+        <f>F3-C3</f>
+        <v>-8.0659872000008903E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>-804510</v>
+      </c>
+      <c r="B4" s="12">
+        <v>11.9</v>
+      </c>
+      <c r="C4" s="13">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <f>(A4-Auswertung!$M$6)/Auswertung!$M$5</f>
+        <v>-0.1465823700000099</v>
+      </c>
+      <c r="E4" s="2">
+        <f>D4-C4</f>
+        <v>-0.1465823700000099</v>
+      </c>
+      <c r="F4" s="6">
+        <f>D4-Auswertung!$K$20*B4-Auswertung!$K$21</f>
+        <v>-1.0926570000009905E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <f>F4-C4</f>
+        <v>-1.0926570000009905E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>-806358</v>
+      </c>
+      <c r="B5" s="12">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="C5" s="13">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <f>(A5-Auswertung!$M$6)/Auswertung!$M$5</f>
+        <v>2.1424853999990102E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <f>D5-C5</f>
+        <v>2.1424853999990102E-2</v>
+      </c>
+      <c r="F5" s="6">
+        <f>D5-Auswertung!$K$20*B5-Auswertung!$K$21</f>
+        <v>-2.2304346000009856E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <f>F5-C5</f>
+        <v>-2.2304346000009856E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>-914010</v>
+      </c>
+      <c r="B6" s="12">
+        <v>20.5</v>
+      </c>
+      <c r="C6" s="13">
+        <v>9.75</v>
+      </c>
+      <c r="D6" s="6">
+        <f>(A6-Auswertung!$M$6)/Auswertung!$M$5</f>
+        <v>9.8083911299999897</v>
+      </c>
+      <c r="E6" s="2">
+        <f>D6-C6</f>
+        <v>5.8391129999989744E-2</v>
+      </c>
+      <c r="F6" s="6">
+        <f>D6-Auswertung!$K$20*B6-Auswertung!$K$21</f>
+        <v>9.7383521299999902</v>
+      </c>
+      <c r="G6" s="2">
+        <f>F6-C6</f>
+        <v>-1.1647870000009775E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>-912120</v>
+      </c>
+      <c r="B7" s="12">
+        <v>12.5</v>
+      </c>
+      <c r="C7" s="13">
+        <v>9.75</v>
+      </c>
+      <c r="D7" s="6">
+        <f>(A7-Auswertung!$M$6)/Auswertung!$M$5</f>
+        <v>9.6365655599999904</v>
+      </c>
+      <c r="E7" s="2">
+        <f>D7-C7</f>
+        <v>-0.11343444000000957</v>
+      </c>
+      <c r="F7" s="6">
+        <f>D7-Auswertung!$K$20*B7-Auswertung!$K$21</f>
+        <v>9.75787055999999</v>
+      </c>
+      <c r="G7" s="2">
+        <f>F7-C7</f>
+        <v>7.8705599999899789E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>-804830</v>
+      </c>
+      <c r="B8" s="12">
+        <v>12.5</v>
+      </c>
+      <c r="C8" s="13">
+        <v>0</v>
+      </c>
+      <c r="D8" s="14">
+        <f>(A8-Auswertung!$M$6)/Auswertung!$M$5</f>
+        <v>-0.11749021000000989</v>
+      </c>
+      <c r="E8" s="8">
+        <f>D8-C8</f>
+        <v>-0.11749021000000989</v>
+      </c>
+      <c r="F8" s="14">
+        <f>D8-Auswertung!$K$20*B8-Auswertung!$K$21</f>
+        <v>3.8147899999900758E-3</v>
+      </c>
+      <c r="G8" s="8">
+        <f>F8-C8</f>
+        <v>3.8147899999900758E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>-805190</v>
+      </c>
+      <c r="B9" s="12">
+        <v>13.9</v>
+      </c>
+      <c r="C9" s="13">
+        <v>0</v>
+      </c>
+      <c r="D9" s="14">
+        <f>(A9-Auswertung!$M$6)/Auswertung!$M$5</f>
+        <v>-8.4761530000009896E-2</v>
+      </c>
+      <c r="E9" s="8">
+        <f>D9-C9</f>
+        <v>-8.4761530000009896E-2</v>
+      </c>
+      <c r="F9" s="14">
+        <f>D9-Auswertung!$K$20*B9-Auswertung!$K$21</f>
+        <v>3.0582699999900931E-3</v>
+      </c>
+      <c r="G9" s="8">
+        <f>F9-C9</f>
+        <v>3.0582699999900931E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>-805850</v>
+      </c>
+      <c r="B10" s="12">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="C10" s="13">
+        <v>0</v>
+      </c>
+      <c r="D10" s="14">
+        <f>(A10-Auswertung!$M$6)/Auswertung!$M$5</f>
+        <v>-2.4758950000009897E-2</v>
+      </c>
+      <c r="E10" s="8">
+        <f>D10-C10</f>
+        <v>-2.4758950000009897E-2</v>
+      </c>
+      <c r="F10" s="14">
+        <f>D10-Auswertung!$K$20*B10-Auswertung!$K$21</f>
+        <v>-1.5177500000099209E-3</v>
+      </c>
+      <c r="G10" s="8">
+        <f>F10-C10</f>
+        <v>-1.5177500000099209E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>-805750</v>
+      </c>
+      <c r="B11" s="12">
+        <v>15.9</v>
+      </c>
+      <c r="C11" s="13">
+        <v>0</v>
+      </c>
+      <c r="D11" s="14">
+        <f>(A11-Auswertung!$M$6)/Auswertung!$M$5</f>
+        <v>-3.3850250000009893E-2</v>
+      </c>
+      <c r="E11" s="8">
+        <f>D11-C11</f>
+        <v>-3.3850250000009893E-2</v>
+      </c>
+      <c r="F11" s="14">
+        <f>D11-Auswertung!$K$20*B11-Auswertung!$K$21</f>
+        <v>6.1335499999901066E-3</v>
+      </c>
+      <c r="G11" s="8">
+        <f>F11-C11</f>
+        <v>6.1335499999901066E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>-806910</v>
+      </c>
+      <c r="B12" s="12">
+        <v>20.5</v>
+      </c>
+      <c r="C12" s="13">
+        <v>0</v>
+      </c>
+      <c r="D12" s="14">
+        <f>(A12-Auswertung!$M$6)/Auswertung!$M$5</f>
+        <v>7.1608829999990103E-2</v>
+      </c>
+      <c r="E12" s="8">
+        <f>D12-C12</f>
+        <v>7.1608829999990103E-2</v>
+      </c>
+      <c r="F12" s="14">
+        <f>D12-Auswertung!$K$20*B12-Auswertung!$K$21</f>
+        <v>1.5698299999901133E-3</v>
+      </c>
+      <c r="G12" s="8">
+        <f>F12-C12</f>
+        <v>1.5698299999901133E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>-807723</v>
+      </c>
+      <c r="B13" s="12">
+        <v>21.9</v>
+      </c>
+      <c r="C13" s="13">
+        <v>0</v>
+      </c>
+      <c r="D13" s="14">
+        <f>(A13-Auswertung!$M$6)/Auswertung!$M$5</f>
+        <v>0.14552109899999011</v>
+      </c>
+      <c r="E13" s="8">
+        <f>D13-C13</f>
+        <v>0.14552109899999011</v>
+      </c>
+      <c r="F13" s="14">
+        <f>D13-Auswertung!$K$20*B13-Auswertung!$K$21</f>
+        <v>4.1996898999990151E-2</v>
+      </c>
+      <c r="G13" s="8">
+        <f>F13-C13</f>
+        <v>4.1996898999990151E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>-808187</v>
+      </c>
+      <c r="B14" s="12">
+        <v>22.8</v>
+      </c>
+      <c r="C14" s="13">
+        <v>0</v>
+      </c>
+      <c r="D14" s="14">
+        <f>(A14-Auswertung!$M$6)/Auswertung!$M$5</f>
+        <v>0.1877047309999901</v>
+      </c>
+      <c r="E14" s="8">
+        <f>D14-C14</f>
+        <v>0.1877047309999901</v>
+      </c>
+      <c r="F14" s="14">
+        <f>D14-Auswertung!$K$20*B14-Auswertung!$K$21</f>
+        <v>6.2654330999990071E-2</v>
+      </c>
+      <c r="G14" s="8">
+        <f>F14-C14</f>
+        <v>6.2654330999990071E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G14">
+    <sortCondition ref="G3:G14"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{190CE8A5-5FE3-40A5-93F7-0F18B64AB58A}">
+  <dimension ref="A2:M33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="4">
+        <v>-9.0913000000000002E-5</v>
+      </c>
+      <c r="L5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="1">
+        <f>1/K5</f>
+        <v>-10999.527020338126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="4">
+        <v>-73.287000000000006</v>
+      </c>
+      <c r="L6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" s="1">
+        <f>-M5*K6</f>
+        <v>-806122.33673952031</v>
+      </c>
+    </row>
+    <row r="17" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+    </row>
+    <row r="19" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+    </row>
+    <row r="20" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="4">
+        <v>2.3917999999999998E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>16</v>
+      </c>
+      <c r="K21" s="4">
+        <v>-0.42027999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="16" t="s">
+    </row>
+    <row r="33" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
         <v>17</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="15"/>
-      <c r="Q2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
-        <v>-43496</v>
-      </c>
-      <c r="B3" s="22">
-        <v>20</v>
-      </c>
-      <c r="C3" s="23">
-        <v>0</v>
-      </c>
-      <c r="D3" s="24">
-        <f t="shared" ref="D3:D10" si="0">(A3-$T$5)/$T$4</f>
-        <v>2.0434399999988672E-4</v>
-      </c>
-      <c r="E3" s="15">
-        <f>D3-C3</f>
-        <v>2.0434399999988672E-4</v>
-      </c>
-      <c r="F3" s="24">
-        <f t="shared" ref="F3:F10" si="1">D3-$R$19*B3-$R$20</f>
-        <v>-4.8496560000001118E-3</v>
-      </c>
-      <c r="G3" s="15">
-        <f>F3-C3</f>
-        <v>-4.8496560000001118E-3</v>
-      </c>
-      <c r="Q3" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
-        <v>108691</v>
-      </c>
-      <c r="B4" s="22">
-        <v>20</v>
-      </c>
-      <c r="C4" s="23">
-        <v>6</v>
-      </c>
-      <c r="D4" s="24">
-        <f t="shared" si="0"/>
-        <v>6.0056555510000003</v>
-      </c>
-      <c r="E4" s="15">
-        <f t="shared" ref="E4:E10" si="2">D4-C4</f>
-        <v>5.6555510000002585E-3</v>
-      </c>
-      <c r="F4" s="24">
-        <f t="shared" si="1"/>
-        <v>6.0006015509999999</v>
-      </c>
-      <c r="G4" s="15">
-        <f t="shared" ref="G4:G10" si="3">F4-C4</f>
-        <v>6.0155099999992245E-4</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>22</v>
-      </c>
-      <c r="R4" s="19">
-        <v>3.9461E-5</v>
-      </c>
-      <c r="S4" t="s">
-        <v>12</v>
-      </c>
-      <c r="T4" s="13">
-        <f>1/R4</f>
-        <v>25341.476394414738</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="18">
-        <v>108000</v>
-      </c>
-      <c r="B5" s="22">
-        <v>0</v>
-      </c>
-      <c r="C5" s="23">
-        <v>6</v>
-      </c>
-      <c r="D5" s="24">
-        <f t="shared" si="0"/>
-        <v>5.9783880000000007</v>
-      </c>
-      <c r="E5" s="15">
-        <f t="shared" si="2"/>
-        <v>-2.1611999999999298E-2</v>
-      </c>
-      <c r="F5" s="24">
-        <f t="shared" si="1"/>
-        <v>5.9983820000000003</v>
-      </c>
-      <c r="G5" s="15">
-        <f t="shared" si="3"/>
-        <v>-1.6179999999996753E-3</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>23</v>
-      </c>
-      <c r="R5" s="19">
-        <v>1.7165999999999999</v>
-      </c>
-      <c r="S5" t="s">
-        <v>11</v>
-      </c>
-      <c r="T5" s="13">
-        <f>-T4*R5</f>
-        <v>-43501.178378652337</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="18">
-        <v>109000</v>
-      </c>
-      <c r="B6" s="22">
-        <v>30</v>
-      </c>
-      <c r="C6" s="23">
-        <v>6</v>
-      </c>
-      <c r="D6" s="24">
-        <f t="shared" si="0"/>
-        <v>6.017849</v>
-      </c>
-      <c r="E6" s="15">
-        <f t="shared" si="2"/>
-        <v>1.7849000000000004E-2</v>
-      </c>
-      <c r="F6" s="24">
-        <f t="shared" si="1"/>
-        <v>6.0002709999999997</v>
-      </c>
-      <c r="G6" s="15">
-        <f t="shared" si="3"/>
-        <v>2.7099999999968816E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
-        <v>108500</v>
-      </c>
-      <c r="B7" s="22">
-        <v>10</v>
-      </c>
-      <c r="C7" s="23">
-        <v>6</v>
-      </c>
-      <c r="D7" s="24">
-        <f t="shared" si="0"/>
-        <v>5.9981185000000004</v>
-      </c>
-      <c r="E7" s="15">
-        <f t="shared" si="2"/>
-        <v>-1.8814999999996473E-3</v>
-      </c>
-      <c r="F7" s="24">
-        <f t="shared" si="1"/>
-        <v>6.0055885</v>
-      </c>
-      <c r="G7" s="15">
-        <f t="shared" si="3"/>
-        <v>5.5884999999999962E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
-        <v>-43000</v>
-      </c>
-      <c r="B8" s="22">
-        <v>30</v>
-      </c>
-      <c r="C8" s="23">
-        <v>0</v>
-      </c>
-      <c r="D8" s="24">
-        <f t="shared" si="0"/>
-        <v>1.9776999999999888E-2</v>
-      </c>
-      <c r="E8" s="15">
-        <f t="shared" si="2"/>
-        <v>1.9776999999999888E-2</v>
-      </c>
-      <c r="F8" s="24">
-        <f t="shared" si="1"/>
-        <v>2.1989999999998885E-3</v>
-      </c>
-      <c r="G8" s="15">
-        <f t="shared" si="3"/>
-        <v>2.1989999999998885E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
-        <v>-43500</v>
-      </c>
-      <c r="B9" s="22">
-        <v>18</v>
-      </c>
-      <c r="C9" s="23">
-        <v>0</v>
-      </c>
-      <c r="D9" s="24">
-        <f t="shared" si="0"/>
-        <v>4.649999999988672E-5</v>
-      </c>
-      <c r="E9" s="15">
-        <f t="shared" si="2"/>
-        <v>4.649999999988672E-5</v>
-      </c>
-      <c r="F9" s="24">
-        <f t="shared" si="1"/>
-        <v>-2.5027000000001146E-3</v>
-      </c>
-      <c r="G9" s="15">
-        <f t="shared" si="3"/>
-        <v>-2.5027000000001146E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="18">
-        <v>-44000</v>
-      </c>
-      <c r="B10" s="22">
-        <v>0</v>
-      </c>
-      <c r="C10" s="23">
-        <v>0</v>
-      </c>
-      <c r="D10" s="24">
-        <f t="shared" si="0"/>
-        <v>-1.9684000000000115E-2</v>
-      </c>
-      <c r="E10" s="15">
-        <f t="shared" si="2"/>
-        <v>-1.9684000000000115E-2</v>
-      </c>
-      <c r="F10" s="24">
-        <f t="shared" si="1"/>
-        <v>3.0999999999988676E-4</v>
-      </c>
-      <c r="G10" s="15">
-        <f t="shared" si="3"/>
-        <v>3.0999999999988676E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="Q17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="Q18" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R18" s="20"/>
-      <c r="S18" s="20"/>
-      <c r="T18" s="20"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="Q19" t="s">
-        <v>24</v>
-      </c>
-      <c r="R19" s="19">
-        <v>1.2524000000000001E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="Q20" t="s">
-        <v>25</v>
-      </c>
-      <c r="R20" s="19">
-        <v>-1.9994000000000001E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="Q32" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q33" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
calibration values as real examples
</commit_message>
<xml_diff>
--- a/docs/Gewicht Eichung Loadcell.xlsx
+++ b/docs/Gewicht Eichung Loadcell.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\beehive-sensor\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FB2FD1-EAC3-4620-96DE-7E82C8490944}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A270C5-E772-4132-BB30-2D6026B6DCDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{8B69D70C-2B63-46EE-9209-063377342C58}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="2" xr2:uid="{8B69D70C-2B63-46EE-9209-063377342C58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -5009,13 +5009,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6393FE46-6FC0-4A51-A64E-4990F17C1E38}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q49" sqref="Q49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -5038,7 +5038,7 @@
         <v>4.4400000000000004</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>171133</v>
       </c>
@@ -5058,7 +5058,7 @@
         <v>63608</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>171225</v>
       </c>
@@ -5078,7 +5078,7 @@
         <v>63701</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>171272</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>63818</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>171336</v>
       </c>
@@ -5118,7 +5118,7 @@
         <v>63835</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>171327</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>63903</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>171157</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>21.87</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>171204</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>21.87</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>171278</v>
       </c>
@@ -5252,7 +5252,7 @@
         <v>21.81</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>171267</v>
       </c>
@@ -5290,7 +5290,7 @@
         <v>21.81</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>171221</v>
       </c>
@@ -5328,7 +5328,7 @@
         <v>21.81</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>171193</v>
       </c>
@@ -5366,7 +5366,7 @@
         <v>21.81</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>171197</v>
       </c>
@@ -5404,7 +5404,7 @@
         <v>21.87</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>171273</v>
       </c>
@@ -5442,7 +5442,7 @@
         <v>21.87</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>171241</v>
       </c>
@@ -5480,7 +5480,7 @@
         <v>21.81</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>171234</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>21.87</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>171215</v>
       </c>
@@ -5556,7 +5556,7 @@
         <v>21.87</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>171269</v>
       </c>
@@ -5594,7 +5594,7 @@
         <v>21.87</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>171388</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>21.87</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>171546</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>21.87</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>171634</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>21.81</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>171747</v>
       </c>
@@ -5731,7 +5731,7 @@
         <v>21.87</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>171766</v>
       </c>
@@ -5763,7 +5763,7 @@
         <v>21.87</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>171782</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>21.87</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>171708</v>
       </c>
@@ -5824,7 +5824,7 @@
         <v>21.87</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -5856,7 +5856,7 @@
         <v>21.87</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -5888,7 +5888,7 @@
         <v>21.87</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -5920,7 +5920,7 @@
         <v>21.81</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -5952,7 +5952,7 @@
         <v>21.87</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -5984,7 +5984,7 @@
         <v>21.87</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -6016,7 +6016,7 @@
         <v>21.87</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -6030,7 +6030,7 @@
         <v>64032</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -6044,7 +6044,7 @@
         <v>64237</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -6058,7 +6058,7 @@
         <v>64089</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -6072,7 +6072,7 @@
         <v>64064</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -6086,7 +6086,7 @@
         <v>64035</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -6115,7 +6115,7 @@
         <v>63970</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -6132,7 +6132,7 @@
         <v>46204</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -6149,7 +6149,7 @@
         <v>10406</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -6158,7 +6158,7 @@
         <v>19557</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>27</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>19839</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>29</v>
       </c>
@@ -6186,17 +6186,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB70EFBE-8999-4967-8E5C-A2958F6E5E70}">
   <dimension ref="A1:O77"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <selection activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -6207,7 +6207,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -6230,7 +6230,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>17725</v>
       </c>
@@ -6257,7 +6257,7 @@
         <v>-1.1046900000000151E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>17653</v>
       </c>
@@ -6284,7 +6284,7 @@
         <v>-1.806229200000015E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>17754</v>
       </c>
@@ -6311,7 +6311,7 @@
         <v>-8.2212560000001506E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>17694</v>
       </c>
@@ -6338,7 +6338,7 @@
         <v>-1.4067416000000152E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>17708</v>
       </c>
@@ -6365,7 +6365,7 @@
         <v>-1.2703312000000151E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>17696</v>
       </c>
@@ -6392,7 +6392,7 @@
         <v>-1.3872544000000151E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>17614</v>
       </c>
@@ -6419,7 +6419,7 @@
         <v>-2.1862296000000152E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>17539</v>
       </c>
@@ -6446,7 +6446,7 @@
         <v>-2.9169996000000149E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>17540</v>
       </c>
@@ -6473,7 +6473,7 @@
         <v>-2.907256000000015E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>17590</v>
       </c>
@@ -6500,7 +6500,7 @@
         <v>-2.4200760000000151E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>17678</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>-1.5626392000000152E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>17743</v>
       </c>
@@ -6561,7 +6561,7 @@
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>17752</v>
       </c>
@@ -6588,7 +6588,7 @@
         <v>-8.4161280000001511E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>17721</v>
       </c>
@@ -6615,7 +6615,7 @@
         <v>-1.1436644000000152E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>17712</v>
       </c>
@@ -6642,7 +6642,7 @@
         <v>-1.2313568000000151E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>17768</v>
       </c>
@@ -6669,7 +6669,7 @@
         <v>-6.8571520000001518E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>17826</v>
       </c>
@@ -6696,7 +6696,7 @@
         <v>-1.2058640000001516E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>17834</v>
       </c>
@@ -6723,7 +6723,7 @@
         <v>-4.2637600000015153E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>17877</v>
       </c>
@@ -6750,7 +6750,7 @@
         <v>3.7633719999998483E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>17851</v>
       </c>
@@ -6777,7 +6777,7 @@
         <v>1.2300359999998483E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>17840</v>
       </c>
@@ -6804,7 +6804,7 @@
         <v>1.5823999999984843E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>17933</v>
       </c>
@@ -6831,7 +6831,7 @@
         <v>9.2197879999998487E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>17961</v>
       </c>
@@ -6858,7 +6858,7 @@
         <v>1.1947995999999848E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>17888</v>
       </c>
@@ -6885,7 +6885,7 @@
         <v>4.8351679999998481E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>17868</v>
       </c>
@@ -6912,7 +6912,7 @@
         <v>2.8864479999998484E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>63903</v>
       </c>
@@ -6939,7 +6939,7 @@
         <v>4.8352707999999467E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>63915</v>
       </c>
@@ -6966,7 +6966,7 @@
         <v>4.9521939999999987E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>63873</v>
       </c>
@@ -6993,7 +6993,7 @@
         <v>4.5429627999999944E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>63942</v>
       </c>
@@ -7020,7 +7020,7 @@
         <v>5.2152711999999823E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>64075</v>
       </c>
@@ -7047,7 +7047,7 @@
         <v>6.5111700000000106E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>63963</v>
       </c>
@@ -7074,7 +7074,7 @@
         <v>5.4198867999999401E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>63898</v>
       </c>
@@ -7101,7 +7101,7 @@
         <v>4.7865527999999991E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>63952</v>
       </c>
@@ -7128,7 +7128,7 @@
         <v>5.3127071999999664E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>63987</v>
       </c>
@@ -7155,7 +7155,7 @@
         <v>5.6537331999999552E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>63947</v>
       </c>
@@ -7182,7 +7182,7 @@
         <v>5.26398919999993E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>63949</v>
       </c>
@@ -7209,7 +7209,7 @@
         <v>5.2834763999999979E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>63832</v>
       </c>
@@ -7236,7 +7236,7 @@
         <v>4.1434751999999797E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>63967</v>
       </c>
@@ -7263,7 +7263,7 @@
         <v>5.458861199999987E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>63995</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>5.7316819999999602E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>63920</v>
       </c>
@@ -7317,7 +7317,7 @@
         <v>5.0009119999999463E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>63985</v>
       </c>
@@ -7344,7 +7344,7 @@
         <v>5.6342459999999761E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>64122</v>
       </c>
@@ -7371,7 +7371,7 @@
         <v>6.9691191999999624E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>63996</v>
       </c>
@@ -7398,7 +7398,7 @@
         <v>5.7414255999999497E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>64139</v>
       </c>
@@ -7425,7 +7425,7 @@
         <v>7.134760399999962E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>64077</v>
       </c>
@@ -7452,7 +7452,7 @@
         <v>6.5306571999999896E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>64135</v>
       </c>
@@ -7479,7 +7479,7 @@
         <v>7.0957860000000039E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>64032</v>
       </c>
@@ -7506,7 +7506,7 @@
         <v>6.0921952000000168E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>64080</v>
       </c>
@@ -7533,7 +7533,7 @@
         <v>6.5598879999999582E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>63932</v>
       </c>
@@ -7560,7 +7560,7 @@
         <v>5.1178351999999983E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>64026</v>
       </c>
@@ -7587,7 +7587,7 @@
         <v>6.0337335999999908E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>72439</v>
       </c>
@@ -7615,7 +7615,7 @@
         <v>-3.9933596000000016E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>72407</v>
       </c>
@@ -7643,7 +7643,7 @@
         <v>-4.3051548000000217E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>72478</v>
       </c>
@@ -7671,7 +7671,7 @@
         <v>-3.6133592000000547E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>72378</v>
       </c>
@@ -7699,7 +7699,7 @@
         <v>-4.5877191999999845E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>72272</v>
       </c>
@@ -7727,7 +7727,7 @@
         <v>-5.620540800000029E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>72292</v>
       </c>
@@ -7755,7 +7755,7 @@
         <v>-5.4256688000000608E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>72486</v>
       </c>
@@ -7783,7 +7783,7 @@
         <v>-3.5354104000000497E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <v>72511</v>
       </c>
@@ -7811,7 +7811,7 @@
         <v>-3.2918204000000451E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>72389</v>
       </c>
@@ -7839,7 +7839,7 @@
         <v>-4.4805396000000108E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>72537</v>
       </c>
@@ -7867,7 +7867,7 @@
         <v>-3.0384868000000509E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>72612</v>
       </c>
@@ -7895,7 +7895,7 @@
         <v>-2.307716800000037E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>72387</v>
       </c>
@@ -7923,7 +7923,7 @@
         <v>-4.5000267999999899E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <v>72531</v>
       </c>
@@ -7951,7 +7951,7 @@
         <v>-3.0969483999999881E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="8">
         <v>72490</v>
       </c>
@@ -7979,7 +7979,7 @@
         <v>-3.4964360000000028E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="8">
         <v>72523</v>
       </c>
@@ -8007,7 +8007,7 @@
         <v>-3.1748971999999931E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
         <v>72238</v>
       </c>
@@ -8035,7 +8035,7 @@
         <v>-5.9518232000000282E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <v>72302</v>
       </c>
@@ -8063,7 +8063,7 @@
         <v>-5.3282327999999879E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <v>72459</v>
       </c>
@@ -8091,7 +8091,7 @@
         <v>-3.7984876000000334E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <v>72438</v>
       </c>
@@ -8119,7 +8119,7 @@
         <v>-4.0031031999999911E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
         <v>72359</v>
       </c>
@@ -8147,7 +8147,7 @@
         <v>-4.7728476000000519E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <v>72239</v>
       </c>
@@ -8175,7 +8175,7 @@
         <v>-5.9420796000000387E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
         <v>72152</v>
       </c>
@@ -8203,7 +8203,7 @@
         <v>-6.7897728000000157E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <v>72084</v>
       </c>
@@ -8231,7 +8231,7 @@
         <v>-7.4523376000000141E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
         <v>72025</v>
       </c>
@@ -8259,7 +8259,7 @@
         <v>-8.0272100000000179E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <v>71925</v>
       </c>
@@ -8300,22 +8300,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{190CE8A5-5FE3-40A5-93F7-0F18B64AB58A}">
   <dimension ref="A2:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="11" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="J2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J3" s="4" t="s">
         <v>19</v>
       </c>
@@ -8323,7 +8323,7 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J4" s="10" t="s">
         <v>18</v>
       </c>
@@ -8331,7 +8331,7 @@
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J5" t="s">
         <v>13</v>
       </c>
@@ -8346,7 +8346,7 @@
         <v>10263.147091424114</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J6" t="s">
         <v>14</v>
       </c>
@@ -8361,12 +8361,12 @@
         <v>17838.375959604255</v>
       </c>
     </row>
-    <row r="17" spans="10:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="10:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J18" s="10" t="s">
         <v>19</v>
       </c>
@@ -8374,7 +8374,7 @@
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="10:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J19" s="10" t="s">
         <v>20</v>
       </c>
@@ -8382,7 +8382,7 @@
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
     </row>
-    <row r="20" spans="10:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J20" t="s">
         <v>15</v>
       </c>
@@ -8390,7 +8390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="10:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J21" t="s">
         <v>16</v>
       </c>
@@ -8398,12 +8398,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="10:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J32" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="10:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J33" t="s">
         <v>17</v>
       </c>

</xml_diff>